<commit_message>
make start epoch and end epoch configurable
</commit_message>
<xml_diff>
--- a/epochscanner.xlsx
+++ b/epochscanner.xlsx
@@ -30,247 +30,247 @@
     <t>Total Number of Epochs</t>
   </si>
   <si>
+    <t>io1qnec80ark9shjc6uzk45dhm8s50dpc27sjuver</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>io1wv5m0xyermvr2n0wjx2cjsqwyk863drdl5qfyn</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>io1wl83n3up9w8nedf30lnyxzple0gu5pme0dyrds</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>io1we5gqn4xeak9ycnu4l9lv0qfq3euapymnzffx6</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>io1c3r4th3zrk4uhv83a9gr4gvn3y6pzaj6mc84ea</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>io15fqav3tugm96ge7anckx0k4gukz5m4mqf0jpv3</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>io1xj0u5n20tsqwxh5a3xdtmzuz9wasft0pqjrq8t</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>io1n3llm0zzlles6pvpzugzajyzyjehztztxf2rff</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>io17cmrextyfeu4gddwd89g5qncedsnc553dhz7xa</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>io1qqaswtu7rcevahucpfxc0zxx088pylwtxnkrrl</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>io159fv8mu9d5djk8u2t0flgw4yqmt6fg98uqjka8</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>io1e3w03ulnrsxth2g0rgsq6v406fhdccsgfq3hz7</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>io1zy9q4myp3jezxdsv82z3f865ruamhqm7a6mggh</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>io13v3dhwds82hg0uc9l4puer00k93qagdh62j0mz</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>io1kugyfdkdss7acy0y9x8fmfjd5qyxfcye3gxt99</t>
+  </si>
+  <si>
+    <t>io17dm3tq9ezgs2uvwrqu8e004l5nqq33jm46r0mg</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>io108h7sa5sap44e244hz649zyk5y4rqzsvnpzxh5</t>
+  </si>
+  <si>
+    <t>io1f0rh94m3ctkwep3rlsswwq5vxwlntx4s574l3q</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>io1nf0rvzgq3tqym6n3trttsrt7d4gqqsmqfzy0da</t>
+  </si>
+  <si>
+    <t>io1sd5t5dwxrk2t50z8yl86n6ht8c99umt4u6rknl</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>io12wc9ra4la98yay4cqdav5mwxxuzwpt6hk23n3z</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>io1aqf30kqz5rqh6zn82c00j684p2h2t5cg30wm8t</t>
+  </si>
+  <si>
+    <t>io1ddjluttkzljqfgdtcz9eu3r3s832umy7ylx0ts</t>
+  </si>
+  <si>
+    <t>io1ar5l5s268rtgzshltnqv88mua06ucm58dx678y</t>
+  </si>
+  <si>
+    <t>io1lm85qfm24eqrc042spnplac9ran28thuh5048n</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>io1gfq9el2gnguus64ex3hu8ajd6e4yzk3f9cz5vx</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>io14u5d66rt465ykm7t2847qllj0reml27q30kr75</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>io1fra0fx6akacny9asewt7vyvggqq4rtq3eznccr</t>
+  </si>
+  <si>
+    <t>io10reczcaelglh5xmkay65h9vw3e5dp82e8vw0rz</t>
+  </si>
+  <si>
+    <t>io12yxdwewry70gr9fs6fphyfaky9c7gurmzk8f4f</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>io1xsx5n94kg2zv64r7tm8vyz9mh86amfak9ka9xx</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>io1kr8c6krd7dhxaaqwdkr6erqgu4z0scug3drgja</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>io1z4sxtefurklkyrfmmdtjmw4h8csnxlv9747hyd</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>io1vtm2zgn830pn6auc2cvnchgwdaefa9gr4z0s86</t>
+  </si>
+  <si>
+    <t>io1u5ff879gg2dw9vfpxr2tsmuaz07e2rea6gvl7s</t>
+  </si>
+  <si>
+    <t>io1rfeltdr5wgmhm4rdx9eun3pp68ahm7fq00wcmm</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>io1vlsmjs87jlk93624nppccfn24nk9nplu9uhu53</t>
+  </si>
+  <si>
+    <t>io1et7zkzc76m9twa4gn5xht3urt9mwj05qvdtj66</t>
+  </si>
+  <si>
+    <t>io1du4eq4f88n4wyc026l3gamjwetlgsg4jz7j884</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>io14vmhs9c75r2ptxdaqrtk0dz7skct30pxmt69d9</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>io1gf08snppu2a2wfd50pjas2j6q2kcxjzqph3pep</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>io1xsdegzr2hdj5sv5ad4nr0yfgpsd98e40u6svem</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>io127ftn4ry6wgxdrw4hcd6gdwqlq70ujk98dvtw5</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>io1zy9q4myp3jezxdsv82z3f865ruamhqm7a6mggh</t>
-  </si>
-  <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>io1qnec80ark9shjc6uzk45dhm8s50dpc27sjuver</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>io1c3r4th3zrk4uhv83a9gr4gvn3y6pzaj6mc84ea</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>io14vmhs9c75r2ptxdaqrtk0dz7skct30pxmt69d9</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>io1vtm2zgn830pn6auc2cvnchgwdaefa9gr4z0s86</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>io15fqav3tugm96ge7anckx0k4gukz5m4mqf0jpv3</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>io1aqf30kqz5rqh6zn82c00j684p2h2t5cg30wm8t</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>io108h7sa5sap44e244hz649zyk5y4rqzsvnpzxh5</t>
-  </si>
-  <si>
-    <t>io1f0rh94m3ctkwep3rlsswwq5vxwlntx4s574l3q</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>io1et7zkzc76m9twa4gn5xht3urt9mwj05qvdtj66</t>
-  </si>
-  <si>
-    <t>io1e3w03ulnrsxth2g0rgsq6v406fhdccsgfq3hz7</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>io1lm85qfm24eqrc042spnplac9ran28thuh5048n</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>io1gfq9el2gnguus64ex3hu8ajd6e4yzk3f9cz5vx</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>io1wl83n3up9w8nedf30lnyxzple0gu5pme0dyrds</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>io1u5ff879gg2dw9vfpxr2tsmuaz07e2rea6gvl7s</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>io1we5gqn4xeak9ycnu4l9lv0qfq3euapymnzffx6</t>
-  </si>
-  <si>
-    <t>io1xsx5n94kg2zv64r7tm8vyz9mh86amfak9ka9xx</t>
-  </si>
-  <si>
-    <t>io1n3llm0zzlles6pvpzugzajyzyjehztztxf2rff</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>io1qqaswtu7rcevahucpfxc0zxx088pylwtxnkrrl</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>io1ddjluttkzljqfgdtcz9eu3r3s832umy7ylx0ts</t>
-  </si>
-  <si>
-    <t>io1z4sxtefurklkyrfmmdtjmw4h8csnxlv9747hyd</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>io1vlsmjs87jlk93624nppccfn24nk9nplu9uhu53</t>
-  </si>
-  <si>
-    <t>io1ar5l5s268rtgzshltnqv88mua06ucm58dx678y</t>
-  </si>
-  <si>
     <t>io1x9kjkr0qv2fa7j4t2as8lrj223xxsqt4tl7xp7</t>
-  </si>
-  <si>
-    <t>io1gf08snppu2a2wfd50pjas2j6q2kcxjzqph3pep</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>io12wc9ra4la98yay4cqdav5mwxxuzwpt6hk23n3z</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>io14u5d66rt465ykm7t2847qllj0reml27q30kr75</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>io1sd5t5dwxrk2t50z8yl86n6ht8c99umt4u6rknl</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>io17cmrextyfeu4gddwd89g5qncedsnc553dhz7xa</t>
-  </si>
-  <si>
-    <t>io1xsdegzr2hdj5sv5ad4nr0yfgpsd98e40u6svem</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>io1kugyfdkdss7acy0y9x8fmfjd5qyxfcye3gxt99</t>
-  </si>
-  <si>
-    <t>io1xj0u5n20tsqwxh5a3xdtmzuz9wasft0pqjrq8t</t>
-  </si>
-  <si>
-    <t>io159fv8mu9d5djk8u2t0flgw4yqmt6fg98uqjka8</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>io12yxdwewry70gr9fs6fphyfaky9c7gurmzk8f4f</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>io13v3dhwds82hg0uc9l4puer00k93qagdh62j0mz</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>io1rfeltdr5wgmhm4rdx9eun3pp68ahm7fq00wcmm</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>io17dm3tq9ezgs2uvwrqu8e004l5nqq33jm46r0mg</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>io1fra0fx6akacny9asewt7vyvggqq4rtq3eznccr</t>
-  </si>
-  <si>
-    <t>io10reczcaelglh5xmkay65h9vw3e5dp82e8vw0rz</t>
-  </si>
-  <si>
-    <t>io1kr8c6krd7dhxaaqwdkr6erqgu4z0scug3drgja</t>
-  </si>
-  <si>
-    <t>io1wv5m0xyermvr2n0wjx2cjsqwyk863drdl5qfyn</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>io1nf0rvzgq3tqym6n3trttsrt7d4gqqsmqfzy0da</t>
-  </si>
-  <si>
-    <t>io1du4eq4f88n4wyc026l3gamjwetlgsg4jz7j884</t>
   </si>
 </sst>
 </file>
@@ -687,10 +687,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -698,10 +698,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -715,10 +715,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -726,13 +726,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -740,13 +740,13 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -754,10 +754,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
@@ -771,7 +771,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>24</v>
@@ -785,10 +785,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -796,13 +796,13 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -810,13 +810,13 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -824,13 +824,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>7</v>
@@ -838,13 +838,13 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>7</v>
@@ -852,13 +852,13 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>7</v>
@@ -866,13 +866,13 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>7</v>
@@ -880,13 +880,13 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>7</v>
@@ -894,13 +894,13 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>7</v>
@@ -908,13 +908,13 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>7</v>
@@ -922,13 +922,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>7</v>
@@ -956,7 +956,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>7</v>
@@ -964,13 +964,13 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>7</v>
@@ -984,7 +984,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>7</v>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>7</v>
@@ -1012,7 +1012,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>7</v>
@@ -1020,13 +1020,13 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>7</v>
@@ -1034,13 +1034,13 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>7</v>
@@ -1048,13 +1048,13 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
@@ -1068,7 +1068,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
@@ -1076,13 +1076,13 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>7</v>
@@ -1093,7 +1093,7 @@
         <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>64</v>
@@ -1107,10 +1107,10 @@
         <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>7</v>
@@ -1118,13 +1118,13 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>7</v>
@@ -1132,13 +1132,13 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>7</v>
@@ -1146,13 +1146,13 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>7</v>
@@ -1180,7 +1180,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>7</v>
@@ -1188,13 +1188,13 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>7</v>
@@ -1202,13 +1202,13 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>7</v>
@@ -1216,13 +1216,13 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>7</v>
@@ -1233,10 +1233,10 @@
         <v>79</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>7</v>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>82</v>
@@ -1261,10 +1261,10 @@
         <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>7</v>
@@ -1275,10 +1275,10 @@
         <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>7</v>

</xml_diff>